<commit_message>
update adcore header mods, css and web ad img doc
</commit_message>
<xml_diff>
--- a/documentation/responsive-web-ad-img-sizes.xlsx
+++ b/documentation/responsive-web-ad-img-sizes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andyedmonds/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andyedmonds/Dropbox/git/repo/agency/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B960B9-AD5E-0144-9DAE-BABFCE831EFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE5DBFC-EEBD-254F-AF22-55B384DAF05A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38600" yWindow="3120" windowWidth="28400" windowHeight="17140" xr2:uid="{8119C1B5-BEF6-C34F-A218-427E1BE9CE33}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>mobile portrait: 0 - 499px</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>600 (393)</t>
+  </si>
+  <si>
+    <t>320 (228)</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,7 +535,7 @@
       <c r="D2" s="1">
         <v>355</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>600</v>
       </c>
       <c r="F2" s="2"/>
@@ -557,8 +560,8 @@
       <c r="D3" s="1">
         <v>355</v>
       </c>
-      <c r="E3" s="2">
-        <v>304</v>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="1" t="s">
@@ -582,8 +585,8 @@
       <c r="D4" s="1">
         <v>355</v>
       </c>
-      <c r="E4" s="2">
-        <v>304</v>
+      <c r="E4" s="1">
+        <v>320</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="1">

</xml_diff>